<commit_message>
explore china energy data
</commit_message>
<xml_diff>
--- a/resources/namelist.xlsx
+++ b/resources/namelist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimim\home\workspace\clj-tinker\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA5F6CB-71C2-4A16-8BF8-E7662B18FF6E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73020A0-AF14-4393-8661-A7A6B70F9155}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14160" xr2:uid="{BCA8E64A-1728-41F9-9676-19BEBC3C2AA8}"/>
   </bookViews>
@@ -54,14 +54,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>James</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UoC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Immo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -79,6 +71,14 @@
   </si>
   <si>
     <t>Ivy Yang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kimi Ma</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZJU</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -449,7 +449,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -470,7 +470,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -484,10 +484,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -532,10 +532,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>33</v>
@@ -546,10 +546,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>34</v>

</xml_diff>